<commit_message>
Committed Excel Data Updated, Abdul Mueed
</commit_message>
<xml_diff>
--- a/Data/Create_Term_Deposits_LCY.xlsx
+++ b/Data/Create_Term_Deposits_LCY.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcelliti6\IdeaProjects\Retail Ops\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xcelliti5\IdeaProjects\Retail Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,25 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Transaction Number</t>
   </si>
   <si>
-    <t>MM2300400041</t>
-  </si>
-  <si>
     <t>MM2300400047</t>
   </si>
   <si>
     <t>MM2300400048</t>
+  </si>
+  <si>
+    <t>MM2300400049</t>
+  </si>
+  <si>
+    <t>MM2300400043</t>
+  </si>
+  <si>
+    <t>MM2316800128</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,17 +369,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>